<commit_message>
Results now are ordered in correct levels
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_ind_effects_hab_season_lmb.xlsx
+++ b/results/accel-glmm-results/glmm_ind_effects_hab_season_lmb.xlsx
@@ -59,13 +59,25 @@
     <t xml:space="preserve">habitat_typeShallow/Low SAV</t>
   </si>
   <si>
+    <t xml:space="preserve">seasonWinter</t>
+  </si>
+  <si>
     <t xml:space="preserve">seasonSpring</t>
   </si>
   <si>
     <t xml:space="preserve">seasonSummer</t>
   </si>
   <si>
-    <t xml:space="preserve">seasonWinter</t>
+    <t xml:space="preserve">habitat_typeExposed/Low SAV:seasonWinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_typeMod/Dense SAV:seasonWinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_typeShallow/Dense SAV:seasonWinter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habitat_typeShallow/Low SAV:seasonWinter</t>
   </si>
   <si>
     <t xml:space="preserve">habitat_typeExposed/Low SAV:seasonSpring</t>
@@ -90,18 +102,6 @@
   </si>
   <si>
     <t xml:space="preserve">habitat_typeShallow/Low SAV:seasonSummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_typeExposed/Low SAV:seasonWinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_typeMod/Dense SAV:seasonWinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_typeShallow/Dense SAV:seasonWinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">habitat_typeShallow/Low SAV:seasonWinter</t>
   </si>
   <si>
     <t xml:space="preserve">ran_pars</t>
@@ -480,16 +480,16 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.23022653385966</v>
+        <v>-1.23854976546635</v>
       </c>
       <c r="F2" t="n">
-        <v>0.069179403760112</v>
+        <v>0.0696205716433035</v>
       </c>
       <c r="G2" t="n">
-        <v>-17.7831329412092</v>
+        <v>-17.7899970688545</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000954916471851954</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000844843248705405</v>
       </c>
     </row>
     <row r="3">
@@ -504,16 +504,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>0.590680896769041</v>
+        <v>0.5907616369183</v>
       </c>
       <c r="F3" t="n">
-        <v>0.200479199438951</v>
+        <v>0.200489652741129</v>
       </c>
       <c r="G3" t="n">
-        <v>2.94634504937213</v>
+        <v>2.94659414509081</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00321553479953186</v>
+        <v>0.00321294597387518</v>
       </c>
     </row>
     <row r="4">
@@ -528,16 +528,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>0.925597791008735</v>
+        <v>0.925588437744798</v>
       </c>
       <c r="F4" t="n">
-        <v>0.383015533322236</v>
+        <v>0.383018311806287</v>
       </c>
       <c r="G4" t="n">
-        <v>2.41660640491574</v>
+        <v>2.41656445452905</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0156659467068363</v>
+        <v>0.0156677520554825</v>
       </c>
     </row>
     <row r="5">
@@ -552,16 +552,16 @@
         <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.155652131614748</v>
+        <v>-0.14850617273924</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0925124947471182</v>
+        <v>0.0926687162520895</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.68249847807284</v>
+        <v>-1.60254915299846</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0924722197925917</v>
+        <v>0.10903422734063</v>
       </c>
     </row>
     <row r="6">
@@ -576,16 +576,16 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>0.233129797590617</v>
+        <v>0.233126748906077</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0216711283447317</v>
+        <v>0.0216718930447652</v>
       </c>
       <c r="G6" t="n">
-        <v>10.7576215636825</v>
+        <v>10.7571013028042</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00000000000000000000000000545601635486561</v>
+        <v>0.00000000000000000000000000548689824848472</v>
       </c>
     </row>
     <row r="7">
@@ -600,16 +600,16 @@
         <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>0.762198325976203</v>
+        <v>-0.239431936597665</v>
       </c>
       <c r="F7" t="n">
-        <v>0.151944893314204</v>
+        <v>0.0366427178206379</v>
       </c>
       <c r="G7" t="n">
-        <v>5.01628129350861</v>
+        <v>-6.5342297416272</v>
       </c>
       <c r="H7" t="n">
-        <v>0.000000526811824600529</v>
+        <v>0.0000000000639377356070636</v>
       </c>
     </row>
     <row r="8">
@@ -624,16 +624,16 @@
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9419047872488</v>
+        <v>0.769476436454697</v>
       </c>
       <c r="F8" t="n">
-        <v>0.022125734303861</v>
+        <v>0.152049489535731</v>
       </c>
       <c r="G8" t="n">
-        <v>42.5705549164276</v>
+        <v>5.0606972690551</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.000000417726013009785</v>
       </c>
     </row>
     <row r="9">
@@ -648,16 +648,16 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.239456257147532</v>
+        <v>0.941956414450631</v>
       </c>
       <c r="F9" t="n">
-        <v>0.036641419955225</v>
+        <v>0.0221266307325715</v>
       </c>
       <c r="G9" t="n">
-        <v>-6.5351249334808</v>
+        <v>42.5711634923262</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0000000000635564647701429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -671,18 +671,10 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" t="n">
-        <v>-0.544089795059353</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.319878467601909</v>
-      </c>
-      <c r="G10" t="n">
-        <v>-1.70092660233848</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.0889567705545069</v>
-      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -695,18 +687,10 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="n">
-        <v>-0.78463972212629</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.44342610920343</v>
-      </c>
-      <c r="G11" t="n">
-        <v>-1.76949373489941</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.0768115153865398</v>
-      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -720,16 +704,16 @@
         <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0125345823598743</v>
+        <v>-0.300353534072304</v>
       </c>
       <c r="F12" t="n">
-        <v>0.156937376742106</v>
+        <v>0.047135774592608</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0798699622746482</v>
+        <v>-6.37209288843228</v>
       </c>
       <c r="H12" t="n">
-        <v>0.936340680117436</v>
+        <v>0.000000000186465887056438</v>
       </c>
     </row>
     <row r="13">
@@ -744,16 +728,16 @@
         <v>21</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.309457079210152</v>
+        <v>-0.358715774094696</v>
       </c>
       <c r="F13" t="n">
-        <v>0.157374787377543</v>
+        <v>0.0427597988870297</v>
       </c>
       <c r="G13" t="n">
-        <v>-1.96637011790054</v>
+        <v>-8.38908936504621</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0492558726124057</v>
+        <v>0.0000000000000000489922192413372</v>
       </c>
     </row>
     <row r="14">
@@ -768,16 +752,16 @@
         <v>22</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.593682979922773</v>
+        <v>-0.544217780925337</v>
       </c>
       <c r="F14" t="n">
-        <v>0.232558130150804</v>
+        <v>0.319889208062018</v>
       </c>
       <c r="G14" t="n">
-        <v>-2.55283691667883</v>
+        <v>-1.70126958712476</v>
       </c>
       <c r="H14" t="n">
-        <v>0.010684951302249</v>
+        <v>0.0888923761087084</v>
       </c>
     </row>
     <row r="15">
@@ -792,16 +776,16 @@
         <v>23</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.95001412011678</v>
+        <v>-0.784634891508651</v>
       </c>
       <c r="F15" t="n">
-        <v>0.395741058565844</v>
+        <v>0.443432840543253</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.40059528712944</v>
+        <v>-1.76945598018268</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0163684285364949</v>
+        <v>0.0768178106557114</v>
       </c>
     </row>
     <row r="16">
@@ -816,16 +800,16 @@
         <v>24</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.00109999522816452</v>
+        <v>0.00536011573658114</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0445415770670036</v>
+        <v>0.157033280891721</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.024695920095281</v>
+        <v>0.0341336289106581</v>
       </c>
       <c r="H16" t="n">
-        <v>0.980297509381816</v>
+        <v>0.972770592108823</v>
       </c>
     </row>
     <row r="17">
@@ -840,16 +824,16 @@
         <v>25</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.349329948631043</v>
+        <v>-0.309461459540699</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0313120260532082</v>
+        <v>0.157380828825096</v>
       </c>
       <c r="G17" t="n">
-        <v>-11.1564147282399</v>
+        <v>-1.96632246666216</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0000000000000000000000000000666245396291721</v>
+        <v>0.0492613732191092</v>
       </c>
     </row>
     <row r="18">
@@ -863,10 +847,18 @@
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
+      <c r="E18" t="n">
+        <v>-0.592272478619254</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.232609096900932</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-2.54621374017673</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0108898487026579</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -879,10 +871,18 @@
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
+      <c r="E19" t="n">
+        <v>-0.948150275482377</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.395753442757862</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-2.39581055536766</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0165836590905726</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -896,16 +896,16 @@
         <v>28</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.300332075863472</v>
+        <v>-0.00105627700287568</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0471341330616956</v>
+        <v>0.0445431552978853</v>
       </c>
       <c r="G20" t="n">
-        <v>-6.37185954964646</v>
+        <v>-0.0237135648745977</v>
       </c>
       <c r="H20" t="n">
-        <v>0.000000000186749873220828</v>
+        <v>0.981081085843704</v>
       </c>
     </row>
     <row r="21">
@@ -920,16 +920,16 @@
         <v>29</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.358696602410278</v>
+        <v>-0.349663006339907</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0427582887162454</v>
+        <v>0.0313162617192958</v>
       </c>
       <c r="G21" t="n">
-        <v>-8.38893728396565</v>
+        <v>-11.1655410685388</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0000000000000000490556295619023</v>
+        <v>0.0000000000000000000000000000601239954249567</v>
       </c>
     </row>
     <row r="22">
@@ -946,7 +946,7 @@
         <v>32</v>
       </c>
       <c r="E22" t="n">
-        <v>0.190421404148217</v>
+        <v>0.189898454364348</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>

</xml_diff>